<commit_message>
fix file paths, update semiology descriptions
</commit_message>
<xml_diff>
--- a/resources/Semiology Descriptions v171.xlsx
+++ b/resources/Semiology Descriptions v171.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{702D81EF-7AE2-424B-9CC6-FD2659E3DEB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242FF1F0-FC31-49A3-8D1E-A10D8CC2200A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="165">
   <si>
     <t>Category</t>
   </si>
@@ -100,9 +100,6 @@
     <t>abdominal aura</t>
   </si>
   <si>
-    <t>cardiovascular e.g. ictal bradycardia</t>
-  </si>
-  <si>
     <t>phosphene</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>large proximal limb or axial movements</t>
   </si>
   <si>
-    <t>psychomotor arrest</t>
-  </si>
-  <si>
     <t>drop attack</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>butterfly sensation</t>
   </si>
   <si>
-    <t>respiratory e.g. hypopnoea</t>
-  </si>
-  <si>
     <t>e.g. people or objects</t>
   </si>
   <si>
@@ -230,9 +221,6 @@
   </si>
   <si>
     <t>rising sensation</t>
-  </si>
-  <si>
-    <t>gastrointestinal: e.g. nausea</t>
   </si>
   <si>
     <t>complex ocular movements</t>
@@ -405,9 +393,6 @@
     <t>tonic and clonic together</t>
   </si>
   <si>
-    <t>movemet of objects (not vestibular)</t>
-  </si>
-  <si>
     <t>macropsia, micropsia</t>
   </si>
   <si>
@@ -513,9 +498,6 @@
     <t>Psychic</t>
   </si>
   <si>
-    <t>Excludes fear/anxiety which has been catagorised separately</t>
-  </si>
-  <si>
     <t>Spasms</t>
   </si>
   <si>
@@ -525,7 +507,17 @@
     <t>Excludes Tonic only and excludes secondarily generalised, therefore few cases</t>
   </si>
   <si>
-    <t>(or during a purposeful behaviour rather than no behaviour)</t>
+    <t xml:space="preserve">cardiovascular e.g. ictal bradycardia, respiratory e.g. hypopnoea, gastrointestinal e.g. nausea
+</t>
+  </si>
+  <si>
+    <t>pain</t>
+  </si>
+  <si>
+    <t>movement of objects (not vestibular)</t>
+  </si>
+  <si>
+    <t>Excludes fear/anxiety which has been categorised separately</t>
   </si>
 </sst>
 </file>
@@ -849,7 +841,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1137,6 +1129,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1182,7 +1183,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1208,15 +1209,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1232,9 +1224,32 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1593,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:E52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1618,7 @@
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.7109375" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -1614,13 +1629,13 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
@@ -1635,16 +1650,16 @@
         <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>134</v>
+        <v>130</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1659,12 +1674,12 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="20" t="s">
-        <v>130</v>
+      <c r="E3" s="17" t="s">
+        <v>125</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1679,14 +1694,14 @@
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="21" t="s">
-        <v>131</v>
+      <c r="E4" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -1701,13 +1716,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -1721,13 +1736,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="20"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1737,20 +1752,20 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>141</v>
+      <c r="A7" s="24" t="s">
+        <v>136</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>143</v>
+        <v>41</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1761,15 +1776,15 @@
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1780,16 +1795,16 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>148</v>
+      <c r="A9" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="20"/>
+        <v>144</v>
+      </c>
+      <c r="E9" s="17"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1799,15 +1814,15 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="20"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -1817,20 +1832,16 @@
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>132</v>
+      <c r="A11" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="17" t="s">
+        <v>127</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1841,13 +1852,11 @@
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="20"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1861,11 +1870,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1875,20 +1884,20 @@
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>151</v>
+        <v>83</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1899,14 +1908,14 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="20" t="s">
-        <v>152</v>
+      <c r="E15" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -1917,20 +1926,20 @@
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>144</v>
+      <c r="A16" s="24" t="s">
+        <v>139</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>145</v>
+        <v>87</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>140</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -1941,19 +1950,17 @@
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>167</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E17" s="32"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1963,20 +1970,20 @@
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>88</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>92</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1991,11 +1998,11 @@
         <v>11</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="20"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -2012,12 +2019,12 @@
         <v>25</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="20"/>
+        <v>66</v>
+      </c>
+      <c r="E20" s="17"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -2027,19 +2034,19 @@
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>153</v>
+      <c r="A21" s="24" t="s">
+        <v>148</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="20"/>
+        <v>67</v>
+      </c>
+      <c r="E21" s="17"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -2049,13 +2056,13 @@
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="20"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -2069,16 +2076,16 @@
         <v>2</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>121</v>
+        <v>74</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>117</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -2090,14 +2097,14 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="20"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -2111,14 +2118,14 @@
         <v>7</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="21" t="s">
-        <v>97</v>
+      <c r="E25" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -2133,14 +2140,14 @@
         <v>8</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="21" t="s">
-        <v>96</v>
+      <c r="E26" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -2155,15 +2162,15 @@
         <v>15</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="20"/>
+        <v>94</v>
+      </c>
+      <c r="E27" s="17"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -2173,14 +2180,14 @@
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>100</v>
+      <c r="A28" s="23" t="s">
+        <v>96</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="24" t="s">
-        <v>101</v>
+      <c r="E28" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -2195,13 +2202,13 @@
         <v>18</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="20"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -2215,11 +2222,11 @@
         <v>20</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="20"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -2230,17 +2237,17 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="20" t="s">
-        <v>159</v>
+      <c r="E31" s="17" t="s">
+        <v>154</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -2255,15 +2262,15 @@
         <v>21</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="20"/>
+        <v>70</v>
+      </c>
+      <c r="E32" s="17"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -2277,11 +2284,11 @@
         <v>14</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="20"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -2292,17 +2299,17 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D34" s="6"/>
-      <c r="E34" s="20" t="s">
-        <v>133</v>
+      <c r="E34" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
@@ -2317,15 +2324,15 @@
         <v>6</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E35" s="20"/>
+        <v>107</v>
+      </c>
+      <c r="E35" s="17"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -2336,14 +2343,14 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="20"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -2354,13 +2361,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="20" t="s">
-        <v>112</v>
+      <c r="E37" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -2372,13 +2379,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="20" t="s">
-        <v>112</v>
+      <c r="E38" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -2390,13 +2397,13 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="20" t="s">
-        <v>112</v>
+      <c r="E39" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -2408,17 +2415,17 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D40" s="6"/>
-      <c r="E40" s="20" t="s">
-        <v>112</v>
+      <c r="E40" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -2430,15 +2437,15 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="20" t="s">
-        <v>112</v>
+      <c r="E41" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -2450,13 +2457,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="20" t="s">
-        <v>112</v>
+      <c r="E42" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -2468,19 +2475,19 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>112</v>
+        <v>69</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -2492,19 +2499,19 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>163</v>
+        <v>120</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -2519,13 +2526,15 @@
         <v>4</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="20"/>
+        <v>49</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" s="17"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -2536,16 +2545,16 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>165</v>
+        <v>68</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>159</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -2560,14 +2569,14 @@
         <v>9</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D47" s="6"/>
-      <c r="E47" s="21" t="s">
-        <v>125</v>
+      <c r="E47" s="18" t="s">
+        <v>121</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -2582,12 +2591,12 @@
         <v>13</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="20" t="s">
-        <v>166</v>
+      <c r="E48" s="17" t="s">
+        <v>160</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -2602,13 +2611,13 @@
         <v>5</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D49" s="6"/>
-      <c r="E49" s="20"/>
+      <c r="E49" s="17"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
@@ -2618,19 +2627,19 @@
       <c r="L49" s="6"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
-        <v>139</v>
+      <c r="A50" s="24" t="s">
+        <v>134</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E50" s="20"/>
+        <v>163</v>
+      </c>
+      <c r="E50" s="17"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -2640,17 +2649,17 @@
       <c r="L50" s="6"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E51" s="20"/>
+        <v>75</v>
+      </c>
+      <c r="E51" s="17"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
@@ -2661,19 +2670,19 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>129</v>
+        <v>71</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
@@ -2696,7 +2705,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I52">
     <sortCondition ref="A2:A52"/>
   </sortState>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="E16:E17"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="B1:D1"/>
@@ -2705,6 +2715,7 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B11:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>